<commit_message>
feat: Add IPA27 CCAA processing notebook, data generation scripts, and analysis figures for indicators, domains, and pillars.
</commit_message>
<xml_diff>
--- a/results/data/auditoria_normalizacion.xlsx
+++ b/results/data/auditoria_normalizacion.xlsx
@@ -2726,10 +2726,10 @@
         <v>9.782345625327082</v>
       </c>
       <c r="Y62">
-        <v>28.53781928734623</v>
+        <v>71.46218071265375</v>
       </c>
       <c r="Z62">
-        <v>26.71287679422889</v>
+        <v>73.2871232057711</v>
       </c>
     </row>
     <row r="63" spans="1:26">
@@ -2767,10 +2767,10 @@
         <v>9.77876167365914</v>
       </c>
       <c r="Y63">
-        <v>27.96861773612405</v>
+        <v>72.03138226387595</v>
       </c>
       <c r="Z63">
-        <v>27.53674471209053</v>
+        <v>72.46325528790946</v>
       </c>
     </row>
     <row r="64" spans="1:26">
@@ -2811,10 +2811,10 @@
         <v>9.734008881819957</v>
       </c>
       <c r="Y64">
-        <v>28.01020128124837</v>
+        <v>71.98979871875164</v>
       </c>
       <c r="Z64">
-        <v>28.09250661213441</v>
+        <v>71.9074933878656</v>
       </c>
     </row>
     <row r="65" spans="1:26">
@@ -2852,10 +2852,10 @@
         <v>9.671739040074923</v>
       </c>
       <c r="Y65">
-        <v>28.68336169528136</v>
+        <v>71.31663830471865</v>
       </c>
       <c r="Z65">
-        <v>28.57695563434786</v>
+        <v>71.42304436565215</v>
       </c>
     </row>
     <row r="66" spans="1:26">
@@ -2896,10 +2896,10 @@
         <v>9.622296451643091</v>
       </c>
       <c r="Y66">
-        <v>30.32467918523953</v>
+        <v>69.67532081476047</v>
       </c>
       <c r="Z66">
-        <v>29.15329093827111</v>
+        <v>70.84670906172889</v>
       </c>
     </row>
     <row r="67" spans="1:26">
@@ -2937,10 +2937,10 @@
         <v>9.59453206152712</v>
       </c>
       <c r="Y67">
-        <v>30.99541216364358</v>
+        <v>69.00458783635642</v>
       </c>
       <c r="Z67">
-        <v>29.52496911392531</v>
+        <v>70.47503088607469</v>
       </c>
     </row>
     <row r="68" spans="1:26">
@@ -2981,10 +2981,10 @@
         <v>9.492735756299361</v>
       </c>
       <c r="Y68">
-        <v>31.03092711969553</v>
+        <v>68.96907288030447</v>
       </c>
       <c r="Z68">
-        <v>30.38888002236865</v>
+        <v>69.61111997763136</v>
       </c>
     </row>
     <row r="69" spans="1:26">
@@ -3022,10 +3022,10 @@
         <v>9.340493710617606</v>
       </c>
       <c r="Y69">
-        <v>30.44898153142136</v>
+        <v>69.55101846857863</v>
       </c>
       <c r="Z69">
-        <v>31.28160822740743</v>
+        <v>68.71839177259255</v>
       </c>
     </row>
     <row r="70" spans="1:26">
@@ -3066,10 +3066,10 @@
         <v>9.197954625702087</v>
       </c>
       <c r="Y70">
-        <v>28.958602604684</v>
+        <v>71.041397395316</v>
       </c>
       <c r="Z70">
-        <v>32.80421281956583</v>
+        <v>67.19578718043418</v>
       </c>
     </row>
     <row r="71" spans="1:26">
@@ -3107,10 +3107,10 @@
         <v>9.024131897832728</v>
       </c>
       <c r="Y71">
-        <v>28.25361274890633</v>
+        <v>71.74638725109367</v>
       </c>
       <c r="Z71">
-        <v>33.82140715825587</v>
+        <v>66.17859284174412</v>
       </c>
     </row>
     <row r="72" spans="1:26">
@@ -3151,10 +3151,10 @@
         <v>8.898335451752898</v>
       </c>
       <c r="Y72">
-        <v>27.98151703619952</v>
+        <v>72.01848296380049</v>
       </c>
       <c r="Z72">
-        <v>34.88861393377896</v>
+        <v>65.11138606622103</v>
       </c>
     </row>
     <row r="73" spans="1:26">
@@ -3192,10 +3192,10 @@
         <v>8.672637094995132</v>
       </c>
       <c r="Y73">
-        <v>28.00626761021015</v>
+        <v>71.99373238978986</v>
       </c>
       <c r="Z73">
-        <v>35.75140893993087</v>
+        <v>64.2485910600691</v>
       </c>
     </row>
     <row r="74" spans="1:26">
@@ -3236,10 +3236,10 @@
         <v>8.54978959976523</v>
       </c>
       <c r="Y74">
-        <v>28.34023975794355</v>
+        <v>71.65976024205645</v>
       </c>
       <c r="Z74">
-        <v>36.78732365033453</v>
+        <v>63.2126763496655</v>
       </c>
     </row>
     <row r="75" spans="1:26">
@@ -3277,10 +3277,10 @@
         <v>8.560621227987257</v>
       </c>
       <c r="Y75">
-        <v>28.68302584345496</v>
+        <v>71.31697415654504</v>
       </c>
       <c r="Z75">
-        <v>36.05057772021189</v>
+        <v>63.9494222797881</v>
       </c>
     </row>
     <row r="76" spans="1:26">
@@ -3321,10 +3321,10 @@
         <v>8.593734120395455</v>
       </c>
       <c r="Y76">
-        <v>29.20601890950007</v>
+        <v>70.79398109049994</v>
       </c>
       <c r="Z76">
-        <v>35.83206563567224</v>
+        <v>64.16793436432775</v>
       </c>
     </row>
     <row r="77" spans="1:26">
@@ -3362,10 +3362,10 @@
         <v>8.600265427877538</v>
       </c>
       <c r="Y77">
-        <v>30.17071548910143</v>
+        <v>69.82928451089857</v>
       </c>
       <c r="Z77">
-        <v>36.07144304843218</v>
+        <v>63.92855695156781</v>
       </c>
     </row>
     <row r="78" spans="1:26">
@@ -3412,10 +3412,10 @@
         <v>8.564923902069875</v>
       </c>
       <c r="Y78">
-        <v>32.05946387205973</v>
+        <v>67.94053612794026</v>
       </c>
       <c r="Z78">
-        <v>34.99810255017731</v>
+        <v>65.00189744982272</v>
       </c>
     </row>
     <row r="79" spans="1:26">
@@ -3459,10 +3459,10 @@
         <v>8.600803701286219</v>
       </c>
       <c r="Y79">
-        <v>33.16946241405981</v>
+        <v>66.83053758594018</v>
       </c>
       <c r="Z79">
-        <v>35.2316112412651</v>
+        <v>64.76838875873489</v>
       </c>
     </row>
     <row r="80" spans="1:26">
@@ -3509,10 +3509,10 @@
         <v>8.650217859154388</v>
       </c>
       <c r="Y80">
-        <v>33.73883101513019</v>
+        <v>66.2611689848698</v>
       </c>
       <c r="Z80">
-        <v>34.82680481286761</v>
+        <v>65.17319518713236</v>
       </c>
     </row>
     <row r="81" spans="1:26">
@@ -3556,10 +3556,10 @@
         <v>8.688235286584778</v>
       </c>
       <c r="Y81">
-        <v>34.23224269875026</v>
+        <v>65.76775730124976</v>
       </c>
       <c r="Z81">
-        <v>34.04464025057709</v>
+        <v>65.9553597494229</v>
       </c>
     </row>
     <row r="82" spans="1:26">
@@ -3606,10 +3606,10 @@
         <v>8.749294922310037</v>
       </c>
       <c r="Y82">
-        <v>35.20584128347129</v>
+        <v>64.79415871652873</v>
       </c>
       <c r="Z82">
-        <v>33.67821529267155</v>
+        <v>66.32178470732846</v>
       </c>
     </row>
     <row r="83" spans="1:26">
@@ -3653,10 +3653,10 @@
         <v>8.802508088951704</v>
       </c>
       <c r="Y83">
-        <v>35.6479263611275</v>
+        <v>64.3520736388725</v>
       </c>
       <c r="Z83">
-        <v>31.48146057834035</v>
+        <v>68.51853942165965</v>
       </c>
     </row>
     <row r="84" spans="1:26">
@@ -3703,10 +3703,10 @@
         <v>8.804017921726235</v>
       </c>
       <c r="Y84">
-        <v>35.95022745070338</v>
+        <v>64.04977254929661</v>
       </c>
       <c r="Z84">
-        <v>31.38472464842286</v>
+        <v>68.61527535157713</v>
       </c>
     </row>
     <row r="85" spans="1:26">
@@ -3750,10 +3750,10 @@
         <v>8.845581487185362</v>
       </c>
       <c r="Y85">
-        <v>35.99600490469785</v>
+        <v>64.00399509530216</v>
       </c>
       <c r="Z85">
-        <v>29.71485071788181</v>
+        <v>70.28514928211817</v>
       </c>
     </row>
     <row r="86" spans="1:26">
@@ -3824,10 +3824,10 @@
         <v>68.40328115703146</v>
       </c>
       <c r="Y86">
-        <v>36.09355592464754</v>
+        <v>63.90644407535245</v>
       </c>
       <c r="Z86">
-        <v>29.5693898912581</v>
+        <v>70.4306101087419</v>
       </c>
     </row>
     <row r="87" spans="1:26">
@@ -3895,10 +3895,10 @@
         <v>67.80760413205135</v>
       </c>
       <c r="Y87">
-        <v>35.98953122128751</v>
+        <v>64.01046877871246</v>
       </c>
       <c r="Z87">
-        <v>29.58163047501864</v>
+        <v>70.41836952498137</v>
       </c>
     </row>
     <row r="88" spans="1:26">
@@ -3969,10 +3969,10 @@
         <v>67.89181492108639</v>
       </c>
       <c r="Y88">
-        <v>35.31085328771176</v>
+        <v>64.68914671228823</v>
       </c>
       <c r="Z88">
-        <v>28.22697047528226</v>
+        <v>71.77302952471774</v>
       </c>
     </row>
     <row r="89" spans="1:26">
@@ -4040,10 +4040,10 @@
         <v>68.69729978983081</v>
       </c>
       <c r="Y89">
-        <v>34.20605956635318</v>
+        <v>65.79394043364684</v>
       </c>
       <c r="Z89">
-        <v>28.29586771566822</v>
+        <v>71.70413228433178</v>
       </c>
     </row>
     <row r="90" spans="1:26">
@@ -4120,10 +4120,10 @@
         <v>69.08241641206548</v>
       </c>
       <c r="Y90">
-        <v>31.96121293011745</v>
+        <v>68.03878706988255</v>
       </c>
       <c r="Z90">
-        <v>26.73524647077147</v>
+        <v>73.26475352922853</v>
       </c>
     </row>
     <row r="91" spans="1:26">
@@ -4197,10 +4197,10 @@
         <v>69.9186516888971</v>
       </c>
       <c r="Y91">
-        <v>30.92795775175549</v>
+        <v>69.0720422482445</v>
       </c>
       <c r="Z91">
-        <v>25.60531963709154</v>
+        <v>74.39468036290846</v>
       </c>
     </row>
     <row r="92" spans="1:26">
@@ -4277,10 +4277,10 @@
         <v>70.19294995251677</v>
       </c>
       <c r="Y92">
-        <v>30.42704097234605</v>
+        <v>69.57295902765397</v>
       </c>
       <c r="Z92">
-        <v>25.11593796177607</v>
+        <v>74.88406203822395</v>
       </c>
     </row>
     <row r="93" spans="1:26">
@@ -4354,10 +4354,10 @@
         <v>70.40598194652068</v>
       </c>
       <c r="Y93">
-        <v>30.68378834578102</v>
+        <v>69.31621165421899</v>
       </c>
       <c r="Z93">
-        <v>24.57757315730402</v>
+        <v>75.42242684269597</v>
       </c>
     </row>
     <row r="94" spans="1:26">
@@ -4434,10 +4434,10 @@
         <v>71.12880435843351</v>
       </c>
       <c r="Y94">
-        <v>31.68689238791426</v>
+        <v>68.31310761208573</v>
       </c>
       <c r="Z94">
-        <v>24.64834115786264</v>
+        <v>75.35165884213735</v>
       </c>
     </row>
     <row r="95" spans="1:26">
@@ -4511,10 +4511,10 @@
         <v>71.11521987522866</v>
       </c>
       <c r="Y95">
-        <v>32.03749907712265</v>
+        <v>67.96250092287735</v>
       </c>
       <c r="Z95">
-        <v>23.39443571272444</v>
+        <v>76.60556428727556</v>
       </c>
     </row>
     <row r="96" spans="1:26">
@@ -4591,10 +4591,10 @@
         <v>71.91682926812685</v>
       </c>
       <c r="Y96">
-        <v>32.11586015743517</v>
+        <v>67.88413984256484</v>
       </c>
       <c r="Z96">
-        <v>22.37644078428707</v>
+        <v>77.62355921571294</v>
       </c>
     </row>
     <row r="97" spans="1:26">
@@ -4668,10 +4668,10 @@
         <v>72.23914649821096</v>
       </c>
       <c r="Y97">
-        <v>32.15974837752792</v>
+        <v>67.8402516224721</v>
       </c>
       <c r="Z97">
-        <v>21.53651860433269</v>
+        <v>78.4634813956673</v>
       </c>
     </row>
     <row r="98" spans="1:26">
@@ -4748,10 +4748,10 @@
         <v>73.03687659437784</v>
       </c>
       <c r="Y98">
-        <v>31.97639261809524</v>
+        <v>68.02360738190477</v>
       </c>
       <c r="Z98">
-        <v>21.0824068134441</v>
+        <v>78.91759318655591</v>
       </c>
     </row>
     <row r="99" spans="1:26">
@@ -4825,10 +4825,10 @@
         <v>73.76667417080809</v>
       </c>
       <c r="Y99">
-        <v>31.70334543104137</v>
+        <v>68.29665456895864</v>
       </c>
       <c r="Z99">
-        <v>21.38291747729888</v>
+        <v>78.61708252270112</v>
       </c>
     </row>
     <row r="100" spans="1:26">
@@ -4905,10 +4905,10 @@
         <v>73.51256425590688</v>
       </c>
       <c r="Y100">
-        <v>31.15803959603971</v>
+        <v>68.84196040396031</v>
       </c>
       <c r="Z100">
-        <v>21.07007538498433</v>
+        <v>78.92992461501566</v>
       </c>
     </row>
     <row r="101" spans="1:26">
@@ -4982,10 +4982,10 @@
         <v>72.88388497890719</v>
       </c>
       <c r="Y101">
-        <v>30.36222235482368</v>
+        <v>69.63777764517633</v>
       </c>
       <c r="Z101">
-        <v>21.11660846562228</v>
+        <v>78.88339153437772</v>
       </c>
     </row>
     <row r="102" spans="1:26">
@@ -5062,10 +5062,10 @@
         <v>72.71228034850854</v>
       </c>
       <c r="Y102">
-        <v>28.66234218916691</v>
+        <v>71.33765781083308</v>
       </c>
       <c r="Z102">
-        <v>21.36407388406427</v>
+        <v>78.63592611593573</v>
       </c>
     </row>
     <row r="103" spans="1:26">
@@ -5139,10 +5139,10 @@
         <v>74.94630872067201</v>
       </c>
       <c r="Y103">
-        <v>28.01023381135517</v>
+        <v>71.98976618864484</v>
       </c>
       <c r="Z103">
-        <v>21.72230101999892</v>
+        <v>78.27769898000108</v>
       </c>
     </row>
     <row r="104" spans="1:26">
@@ -5219,10 +5219,10 @@
         <v>70.30638271017447</v>
       </c>
       <c r="Y104">
-        <v>28.12805706593276</v>
+        <v>71.87194293406725</v>
       </c>
       <c r="Z104">
-        <v>22.90620611170231</v>
+        <v>77.0937938882977</v>
       </c>
     </row>
     <row r="105" spans="1:26">
@@ -5296,10 +5296,10 @@
         <v>70.84502822064493</v>
       </c>
       <c r="Y105">
-        <v>29.19936693354516</v>
+        <v>70.80063306645484</v>
       </c>
       <c r="Z105">
-        <v>22.97129934899959</v>
+        <v>77.02870065100041</v>
       </c>
     </row>
     <row r="106" spans="1:26">
@@ -5376,10 +5376,10 @@
         <v>71.13871267946899</v>
       </c>
       <c r="Y106">
-        <v>31.6895901899506</v>
+        <v>68.31040981004939</v>
       </c>
       <c r="Z106">
-        <v>22.97948634359463</v>
+        <v>77.02051365640538</v>
       </c>
     </row>
     <row r="107" spans="1:26">
@@ -5456,10 +5456,10 @@
         <v>70.89480447473635</v>
       </c>
       <c r="Y107">
-        <v>32.73691750185914</v>
+        <v>67.26308249814085</v>
       </c>
       <c r="Z107">
-        <v>22.25561728134645</v>
+        <v>77.74438271865355</v>
       </c>
     </row>
     <row r="108" spans="1:26">
@@ -5536,10 +5536,10 @@
         <v>71.50702099223805</v>
       </c>
       <c r="Y108">
-        <v>32.7924589314801</v>
+        <v>67.20754106851989</v>
       </c>
       <c r="Z108">
-        <v>21.77524068779275</v>
+        <v>78.22475931220724</v>
       </c>
     </row>
     <row r="109" spans="1:26">
@@ -5616,10 +5616,10 @@
         <v>70.87946185355655</v>
       </c>
       <c r="Y109">
-        <v>31.98103337671015</v>
+        <v>68.01896662328986</v>
       </c>
       <c r="Z109">
-        <v>20.40623281534728</v>
+        <v>79.59376718465271</v>
       </c>
     </row>
     <row r="110" spans="1:26">
@@ -5696,10 +5696,10 @@
         <v>70.33815642695495</v>
       </c>
       <c r="Y110">
-        <v>29.92312796901665</v>
+        <v>70.07687203098334</v>
       </c>
       <c r="Z110">
-        <v>19.69928811989992</v>
+        <v>80.3007118801001</v>
       </c>
     </row>
     <row r="111" spans="1:26">
@@ -5776,10 +5776,10 @@
         <v>70.30882069235413</v>
       </c>
       <c r="Y111">
-        <v>28.88993859698963</v>
+        <v>71.11006140301038</v>
       </c>
       <c r="Z111">
-        <v>19.22976537911493</v>
+        <v>80.77023462088506</v>
       </c>
     </row>
     <row r="112" spans="1:26">
@@ -5856,10 +5856,10 @@
         <v>69.8325001055704</v>
       </c>
       <c r="Y112">
-        <v>28.57881065873526</v>
+        <v>71.42118934126475</v>
       </c>
       <c r="Z112">
-        <v>18.48170026740122</v>
+        <v>81.51829973259879</v>
       </c>
     </row>
     <row r="113" spans="1:26">
@@ -5936,10 +5936,10 @@
         <v>69.55052277512048</v>
       </c>
       <c r="Y113">
-        <v>29.00812277525846</v>
+        <v>70.99187722474154</v>
       </c>
       <c r="Z113">
-        <v>19.13108008889459</v>
+        <v>80.86891991110541</v>
       </c>
     </row>
     <row r="114" spans="1:26">
@@ -6016,10 +6016,10 @@
         <v>68.48298350082278</v>
       </c>
       <c r="Y114">
-        <v>30.22587477987253</v>
+        <v>69.77412522012746</v>
       </c>
       <c r="Z114">
-        <v>18.32058864251125</v>
+        <v>81.67941135748876</v>
       </c>
     </row>
     <row r="115" spans="1:26">
@@ -6096,10 +6096,10 @@
         <v>68.67681959561826</v>
       </c>
       <c r="Y115">
-        <v>30.71243596081413</v>
+        <v>69.28756403918585</v>
       </c>
       <c r="Z115">
-        <v>18.66083184071266</v>
+        <v>81.33916815928733</v>
       </c>
     </row>
     <row r="116" spans="1:26">
@@ -6176,10 +6176,10 @@
         <v>69.23473682212983</v>
       </c>
       <c r="Y116">
-        <v>30.71356737329746</v>
+        <v>69.28643262670253</v>
       </c>
       <c r="Z116">
-        <v>18.40190604394134</v>
+        <v>81.59809395605869</v>
       </c>
     </row>
     <row r="117" spans="1:26">
@@ -6256,10 +6256,10 @@
         <v>69.24546008142913</v>
       </c>
       <c r="Y117">
-        <v>30.34812188601589</v>
+        <v>69.65187811398414</v>
       </c>
       <c r="Z117">
-        <v>17.70271529364888</v>
+        <v>82.29728470635108</v>
       </c>
     </row>
     <row r="118" spans="1:26">
@@ -6336,10 +6336,10 @@
         <v>69.42067463403771</v>
       </c>
       <c r="Y118">
-        <v>29.78157199368574</v>
+        <v>70.21842800631427</v>
       </c>
       <c r="Z118">
-        <v>17.4911928176524</v>
+        <v>82.50880718234761</v>
       </c>
     </row>
     <row r="119" spans="1:26">
@@ -6416,10 +6416,10 @@
         <v>69.56501687423558</v>
       </c>
       <c r="Y119">
-        <v>29.40576241464327</v>
+        <v>70.59423758535672</v>
       </c>
       <c r="Z119">
-        <v>16.72059794091884</v>
+        <v>83.27940205908116</v>
       </c>
     </row>
     <row r="120" spans="1:26">
@@ -6496,10 +6496,10 @@
         <v>69.68392641682297</v>
       </c>
       <c r="Y120">
-        <v>29.01418487379162</v>
+        <v>70.98581512620839</v>
       </c>
       <c r="Z120">
-        <v>15.89334539193414</v>
+        <v>84.10665460806591</v>
       </c>
     </row>
     <row r="121" spans="1:26">
@@ -6576,10 +6576,10 @@
         <v>69.78188443173917</v>
       </c>
       <c r="Y121">
-        <v>28.59848071787937</v>
+        <v>71.40151928212063</v>
       </c>
       <c r="Z121">
-        <v>15.8825164889213</v>
+        <v>84.11748351107862</v>
       </c>
     </row>
     <row r="122" spans="1:26">
@@ -6656,10 +6656,10 @@
         <v>69.86258251935709</v>
       </c>
       <c r="Y122">
-        <v>28.01451480704692</v>
+        <v>71.98548519295302</v>
       </c>
       <c r="Z122">
-        <v>15.62426722558767</v>
+        <v>84.37573277441234</v>
       </c>
     </row>
     <row r="123" spans="1:26">
@@ -6736,10 +6736,10 @@
         <v>69.9290618304248</v>
       </c>
       <c r="Y123">
-        <v>27.73532021312128</v>
+        <v>72.26467978687867</v>
       </c>
       <c r="Z123">
-        <v>15.30530707470979</v>
+        <v>84.69469292529023</v>
       </c>
     </row>
     <row r="124" spans="1:26">
@@ -6816,10 +6816,10 @@
         <v>69.98382767346388</v>
       </c>
       <c r="Y124">
-        <v>27.40472406123003</v>
+        <v>72.59527593876999</v>
       </c>
       <c r="Z124">
-        <v>15.29891447149877</v>
+        <v>84.70108552850131</v>
       </c>
     </row>
     <row r="125" spans="1:26">
@@ -6896,10 +6896,10 @@
         <v>70.02894392866583</v>
       </c>
       <c r="Y125">
-        <v>27.64544091860177</v>
+        <v>72.35455908139829</v>
       </c>
       <c r="Z125">
-        <v>14.82680246204483</v>
+        <v>85.17319753795506</v>
       </c>
     </row>
   </sheetData>
@@ -7765,10 +7765,10 @@
         <v>67.89285931692665</v>
       </c>
       <c r="Y62">
-        <v>0</v>
+        <v>78.08109548472896</v>
       </c>
       <c r="Z62">
-        <v>0</v>
+        <v>76.01507500378794</v>
       </c>
     </row>
     <row r="63" spans="1:26">
@@ -7806,10 +7806,10 @@
         <v>67.86798545377462</v>
       </c>
       <c r="Y63">
-        <v>0.9529137100933283</v>
+        <v>78.7030171813218</v>
       </c>
       <c r="Z63">
-        <v>0</v>
+        <v>75.16054041667326</v>
       </c>
     </row>
     <row r="64" spans="1:26">
@@ -7850,10 +7850,10 @@
         <v>67.55738561231013</v>
       </c>
       <c r="Y64">
-        <v>0.805651195333823</v>
+        <v>78.65758211727722</v>
       </c>
       <c r="Z64">
-        <v>0</v>
+        <v>74.58409150357478</v>
       </c>
     </row>
     <row r="65" spans="1:26">
@@ -7891,10 +7891,10 @@
         <v>67.12521139078834</v>
       </c>
       <c r="Y65">
-        <v>0</v>
+        <v>77.92207276057293</v>
       </c>
       <c r="Z65">
-        <v>0</v>
+        <v>74.0816099331675</v>
       </c>
     </row>
     <row r="66" spans="1:26">
@@ -7935,10 +7935,10 @@
         <v>66.78206274022584</v>
       </c>
       <c r="Y66">
-        <v>0</v>
+        <v>76.12873443285676</v>
       </c>
       <c r="Z66">
-        <v>0</v>
+        <v>73.48382181652865</v>
       </c>
     </row>
     <row r="67" spans="1:26">
@@ -7976,10 +7976,10 @@
         <v>66.58936827773582</v>
       </c>
       <c r="Y67">
-        <v>0</v>
+        <v>75.39587734384479</v>
       </c>
       <c r="Z67">
-        <v>0</v>
+        <v>73.09830873914535</v>
       </c>
     </row>
     <row r="68" spans="1:26">
@@ -8020,10 +8020,10 @@
         <v>65.88286673970821</v>
       </c>
       <c r="Y68">
-        <v>0</v>
+        <v>75.35707294903099</v>
       </c>
       <c r="Z68">
-        <v>0</v>
+        <v>72.20224064929108</v>
       </c>
     </row>
     <row r="69" spans="1:26">
@@ -8061,10 +8061,10 @@
         <v>64.82625432940536</v>
       </c>
       <c r="Y69">
-        <v>0</v>
+        <v>75.99291905100849</v>
       </c>
       <c r="Z69">
-        <v>0</v>
+        <v>71.27628260242538</v>
       </c>
     </row>
     <row r="70" spans="1:26">
@@ -8105,10 +8105,10 @@
         <v>63.83698382006274</v>
       </c>
       <c r="Y70">
-        <v>0</v>
+        <v>77.62133870076599</v>
       </c>
       <c r="Z70">
-        <v>0</v>
+        <v>69.6970024067891</v>
       </c>
     </row>
     <row r="71" spans="1:26">
@@ -8146,10 +8146,10 @@
         <v>62.63059401731804</v>
       </c>
       <c r="Y71">
-        <v>0</v>
+        <v>78.39162558112417</v>
       </c>
       <c r="Z71">
-        <v>0</v>
+        <v>68.64194524849606</v>
       </c>
     </row>
     <row r="72" spans="1:26">
@@ -8190,10 +8190,10 @@
         <v>61.75752320757739</v>
       </c>
       <c r="Y72">
-        <v>0.9072325792019553</v>
+        <v>78.68892313226208</v>
       </c>
       <c r="Z72">
-        <v>0</v>
+        <v>67.53501405052606</v>
       </c>
     </row>
     <row r="73" spans="1:26">
@@ -8231,10 +8231,10 @@
         <v>60.191098612668</v>
       </c>
       <c r="Y73">
-        <v>0.8195817605992972</v>
+        <v>78.66188012974867</v>
       </c>
       <c r="Z73">
-        <v>0</v>
+        <v>66.64010339996899</v>
       </c>
     </row>
     <row r="74" spans="1:26">
@@ -8275,10 +8275,10 @@
         <v>59.33849454095268</v>
       </c>
       <c r="Y74">
-        <v>0</v>
+        <v>78.29697507232723</v>
       </c>
       <c r="Z74">
-        <v>0</v>
+        <v>65.56562904534381</v>
       </c>
     </row>
     <row r="75" spans="1:26">
@@ -8316,10 +8316,10 @@
         <v>59.41366978411187</v>
       </c>
       <c r="Y75">
-        <v>0</v>
+        <v>77.92243971940714</v>
       </c>
       <c r="Z75">
-        <v>0</v>
+        <v>66.32979872055074</v>
       </c>
     </row>
     <row r="76" spans="1:26">
@@ -8360,10 +8360,10 @@
         <v>59.64348470089684</v>
       </c>
       <c r="Y76">
-        <v>0</v>
+        <v>77.35100639452838</v>
       </c>
       <c r="Z76">
-        <v>0</v>
+        <v>66.55644443631829</v>
       </c>
     </row>
     <row r="77" spans="1:26">
@@ -8401,10 +8401,10 @@
         <v>59.6888142319746</v>
       </c>
       <c r="Y77">
-        <v>0</v>
+        <v>76.29695843525154</v>
       </c>
       <c r="Z77">
-        <v>0</v>
+        <v>66.30815672642866</v>
       </c>
     </row>
     <row r="78" spans="1:26">
@@ -8451,10 +8451,10 @@
         <v>59.44353182920477</v>
       </c>
       <c r="Y78">
-        <v>0</v>
+        <v>74.23327186193819</v>
       </c>
       <c r="Z78">
-        <v>0</v>
+        <v>67.42144996145394</v>
       </c>
     </row>
     <row r="79" spans="1:26">
@@ -8498,10 +8498,10 @@
         <v>59.69255003545256</v>
       </c>
       <c r="Y79">
-        <v>0</v>
+        <v>73.02046389440198</v>
       </c>
       <c r="Z79">
-        <v>0</v>
+        <v>67.17924942347895</v>
       </c>
     </row>
     <row r="80" spans="1:26">
@@ -8548,10 +8548,10 @@
         <v>60.03550136807794</v>
       </c>
       <c r="Y80">
-        <v>0</v>
+        <v>72.39835967559929</v>
       </c>
       <c r="Z80">
-        <v>0</v>
+        <v>67.59912387987222</v>
       </c>
     </row>
     <row r="81" spans="1:26">
@@ -8595,10 +8595,10 @@
         <v>60.29935545287334</v>
       </c>
       <c r="Y81">
-        <v>0</v>
+        <v>71.85924759704506</v>
       </c>
       <c r="Z81">
-        <v>0</v>
+        <v>68.41040279582697</v>
       </c>
     </row>
     <row r="82" spans="1:26">
@@ -8645,10 +8645,10 @@
         <v>60.72313042638326</v>
       </c>
       <c r="Y82">
-        <v>0</v>
+        <v>70.79547311802277</v>
       </c>
       <c r="Z82">
-        <v>0</v>
+        <v>68.79046711599744</v>
       </c>
     </row>
     <row r="83" spans="1:26">
@@ -8692,10 +8692,10 @@
         <v>61.09244819279473</v>
       </c>
       <c r="Y83">
-        <v>0</v>
+        <v>70.31244157859008</v>
       </c>
       <c r="Z83">
-        <v>0</v>
+        <v>71.06899118776317</v>
       </c>
     </row>
     <row r="84" spans="1:26">
@@ -8742,10 +8742,10 @@
         <v>61.10292695403251</v>
       </c>
       <c r="Y84">
-        <v>0</v>
+        <v>69.98214099155336</v>
       </c>
       <c r="Z84">
-        <v>0</v>
+        <v>71.16932789967902</v>
       </c>
     </row>
     <row r="85" spans="1:26">
@@ -8789,10 +8789,10 @@
         <v>61.39139246225586</v>
       </c>
       <c r="Y85">
-        <v>0</v>
+        <v>69.93212357365843</v>
       </c>
       <c r="Z85">
-        <v>0</v>
+        <v>72.90135921056218</v>
       </c>
     </row>
     <row r="86" spans="1:26">
@@ -8863,10 +8863,10 @@
         <v>91.14477737005537</v>
       </c>
       <c r="Y86">
-        <v>0</v>
+        <v>69.82553725866823</v>
       </c>
       <c r="Z86">
-        <v>0</v>
+        <v>73.05223449618187</v>
       </c>
     </row>
     <row r="87" spans="1:26">
@@ -8934,10 +8934,10 @@
         <v>90.35106033034744</v>
       </c>
       <c r="Y87">
-        <v>0</v>
+        <v>69.93919685756129</v>
       </c>
       <c r="Z87">
-        <v>0</v>
+        <v>73.03953828364212</v>
       </c>
     </row>
     <row r="88" spans="1:26">
@@ -9008,10 +9008,10 @@
         <v>90.4632680123318</v>
       </c>
       <c r="Y88">
-        <v>0</v>
+        <v>70.68073477323149</v>
       </c>
       <c r="Z88">
-        <v>0</v>
+        <v>74.44462251918328</v>
       </c>
     </row>
     <row r="89" spans="1:26">
@@ -9079,10 +9079,10 @@
         <v>91.53654604512265</v>
       </c>
       <c r="Y89">
-        <v>0</v>
+        <v>71.88785584325862</v>
       </c>
       <c r="Z89">
-        <v>0</v>
+        <v>74.37316073072164</v>
       </c>
     </row>
     <row r="90" spans="1:26">
@@ -9159,10 +9159,10 @@
         <v>92.04969933545247</v>
       </c>
       <c r="Y90">
-        <v>0</v>
+        <v>74.34062292655385</v>
       </c>
       <c r="Z90">
-        <v>0</v>
+        <v>75.99187266528956</v>
       </c>
     </row>
     <row r="91" spans="1:26">
@@ -9236,10 +9236,10 @@
         <v>93.16395112055079</v>
       </c>
       <c r="Y91">
-        <v>0</v>
+        <v>75.4695794660439</v>
       </c>
       <c r="Z91">
-        <v>0</v>
+        <v>77.16385853748449</v>
       </c>
     </row>
     <row r="92" spans="1:26">
@@ -9316,10 +9316,10 @@
         <v>93.52944315174757</v>
       </c>
       <c r="Y92">
-        <v>0</v>
+        <v>76.01689177155893</v>
       </c>
       <c r="Z92">
-        <v>0</v>
+        <v>77.67145636814482</v>
       </c>
     </row>
     <row r="93" spans="1:26">
@@ -9393,10 +9393,10 @@
         <v>93.81330020272163</v>
       </c>
       <c r="Y93">
-        <v>0</v>
+        <v>75.73636414168938</v>
       </c>
       <c r="Z93">
-        <v>0</v>
+        <v>78.22986061709368</v>
       </c>
     </row>
     <row r="94" spans="1:26">
@@ -9473,10 +9473,10 @@
         <v>94.77643364745566</v>
       </c>
       <c r="Y94">
-        <v>0</v>
+        <v>74.64035137362315</v>
       </c>
       <c r="Z94">
-        <v>0</v>
+        <v>78.15645843353099</v>
       </c>
     </row>
     <row r="95" spans="1:26">
@@ -9550,10 +9550,10 @@
         <v>94.75833283889136</v>
       </c>
       <c r="Y95">
-        <v>0</v>
+        <v>74.25727106310561</v>
       </c>
       <c r="Z95">
-        <v>0</v>
+        <v>79.45703774802007</v>
       </c>
     </row>
     <row r="96" spans="1:26">
@@ -9630,10 +9630,10 @@
         <v>95.82644694712724</v>
       </c>
       <c r="Y96">
-        <v>0</v>
+        <v>74.17165208348379</v>
       </c>
       <c r="Z96">
-        <v>0</v>
+        <v>80.51292529625104</v>
       </c>
     </row>
     <row r="97" spans="1:26">
@@ -9707,10 +9707,10 @@
         <v>96.25592242961335</v>
       </c>
       <c r="Y97">
-        <v>0</v>
+        <v>74.12369888265025</v>
       </c>
       <c r="Z97">
-        <v>0.2331166225665426</v>
+        <v>81.38411173001664</v>
       </c>
     </row>
     <row r="98" spans="1:26">
@@ -9787,10 +9787,10 @@
         <v>97.31886752210983</v>
       </c>
       <c r="Y98">
-        <v>0</v>
+        <v>74.32403727726913</v>
       </c>
       <c r="Z98">
-        <v>2.336767584648447</v>
+        <v>81.8551268324594</v>
       </c>
     </row>
     <row r="99" spans="1:26">
@@ -9864,10 +9864,10 @@
         <v>98.29129510897133</v>
       </c>
       <c r="Y99">
-        <v>0</v>
+        <v>74.62237442947439</v>
       </c>
       <c r="Z99">
-        <v>0.9446664328660148</v>
+        <v>81.54343032080591</v>
       </c>
     </row>
     <row r="100" spans="1:26">
@@ -9944,10 +9944,10 @@
         <v>97.95270328662841</v>
       </c>
       <c r="Y100">
-        <v>0</v>
+        <v>75.21818715932027</v>
       </c>
       <c r="Z100">
-        <v>2.393892332042658</v>
+        <v>81.8679172711923</v>
       </c>
     </row>
     <row r="101" spans="1:26">
@@ -10021,10 +10021,10 @@
         <v>97.11501199799328</v>
       </c>
       <c r="Y101">
-        <v>0</v>
+        <v>76.08771396888736</v>
       </c>
       <c r="Z101">
-        <v>2.178330081035873</v>
+        <v>81.81965209908397</v>
       </c>
     </row>
     <row r="102" spans="1:26">
@@ -10101,10 +10101,10 @@
         <v>96.88635533754086</v>
       </c>
       <c r="Y102">
-        <v>0</v>
+        <v>77.94503911910824</v>
       </c>
       <c r="Z102">
-        <v>1.031958469391892</v>
+        <v>81.56297532530891</v>
       </c>
     </row>
     <row r="103" spans="1:26">
@@ -10178,10 +10178,10 @@
         <v>99.86311339906983</v>
       </c>
       <c r="Y103">
-        <v>0.8055359943494156</v>
+        <v>78.65754657419204</v>
       </c>
       <c r="Z103">
-        <v>0</v>
+        <v>81.19141397298229</v>
       </c>
     </row>
     <row r="104" spans="1:26">
@@ -10258,10 +10258,10 @@
         <v>93.68058799843188</v>
       </c>
       <c r="Y104">
-        <v>0.3882808345411104</v>
+        <v>78.52881038535412</v>
       </c>
       <c r="Z104">
-        <v>0</v>
+        <v>79.96344062095811</v>
       </c>
     </row>
     <row r="105" spans="1:26">
@@ -10335,10 +10335,10 @@
         <v>94.39831270845718</v>
       </c>
       <c r="Y105">
-        <v>0</v>
+        <v>77.35827448464985</v>
       </c>
       <c r="Z105">
-        <v>0</v>
+        <v>79.89592443122449</v>
       </c>
     </row>
     <row r="106" spans="1:26">
@@ -10415,10 +10415,10 @@
         <v>94.78963610937875</v>
       </c>
       <c r="Y106">
-        <v>0</v>
+        <v>74.63740369785539</v>
       </c>
       <c r="Z106">
-        <v>0</v>
+        <v>79.88743269378176</v>
       </c>
     </row>
     <row r="107" spans="1:26">
@@ -10495,10 +10495,10 @@
         <v>94.4646376788495</v>
       </c>
       <c r="Y107">
-        <v>0</v>
+        <v>73.49307164656081</v>
       </c>
       <c r="Z107">
-        <v>0</v>
+        <v>80.63824618805988</v>
       </c>
     </row>
     <row r="108" spans="1:26">
@@ -10575,10 +10575,10 @@
         <v>95.28039296494264</v>
       </c>
       <c r="Y108">
-        <v>0</v>
+        <v>73.43238590164867</v>
       </c>
       <c r="Z108">
-        <v>0</v>
+        <v>81.13650374261718</v>
       </c>
     </row>
     <row r="109" spans="1:26">
@@ -10655,10 +10655,10 @@
         <v>94.4441942181258</v>
       </c>
       <c r="Y109">
-        <v>0</v>
+        <v>74.31896668590292</v>
       </c>
       <c r="Z109">
-        <v>5.469111007944649</v>
+        <v>82.55646991883793</v>
       </c>
     </row>
     <row r="110" spans="1:26">
@@ -10735,10 +10735,10 @@
         <v>93.72292527075552</v>
       </c>
       <c r="Y110">
-        <v>0</v>
+        <v>76.56747781492592</v>
       </c>
       <c r="Z110">
-        <v>8.743998202145276</v>
+        <v>83.28972907402513</v>
       </c>
     </row>
     <row r="111" spans="1:26">
@@ -10815,10 +10815,10 @@
         <v>93.68383651720522</v>
       </c>
       <c r="Y111">
-        <v>0</v>
+        <v>77.69636245301766</v>
       </c>
       <c r="Z111">
-        <v>10.91903964610108</v>
+        <v>83.77672876504238</v>
       </c>
     </row>
     <row r="112" spans="1:26">
@@ -10895,10 +10895,10 @@
         <v>93.04915740379379</v>
       </c>
       <c r="Y112">
-        <v>0</v>
+        <v>78.03630744227692</v>
       </c>
       <c r="Z112">
-        <v>14.384415184748</v>
+        <v>84.55263895345264</v>
       </c>
     </row>
     <row r="113" spans="1:26">
@@ -10975,10 +10975,10 @@
         <v>92.67343330733912</v>
       </c>
       <c r="Y113">
-        <v>0</v>
+        <v>77.5672319112938</v>
       </c>
       <c r="Z113">
-        <v>11.37619449184761</v>
+        <v>83.87908739790628</v>
       </c>
     </row>
     <row r="114" spans="1:26">
@@ -11055,10 +11055,10 @@
         <v>91.25097771977332</v>
       </c>
       <c r="Y114">
-        <v>0</v>
+        <v>76.23669022335793</v>
       </c>
       <c r="Z114">
-        <v>15.1307570140125</v>
+        <v>84.71974760384417</v>
       </c>
     </row>
     <row r="115" spans="1:26">
@@ -11135,10 +11135,10 @@
         <v>91.5092569632186</v>
       </c>
       <c r="Y115">
-        <v>0</v>
+        <v>75.70506314943718</v>
       </c>
       <c r="Z115">
-        <v>13.55459681381669</v>
+        <v>84.3668396017359</v>
       </c>
     </row>
     <row r="116" spans="1:26">
@@ -11215,10 +11215,10 @@
         <v>92.25266050382625</v>
       </c>
       <c r="Y116">
-        <v>0</v>
+        <v>75.70382694414283</v>
       </c>
       <c r="Z116">
-        <v>14.75405807515059</v>
+        <v>84.63540334119021</v>
       </c>
     </row>
     <row r="117" spans="1:26">
@@ -11295,10 +11295,10 @@
         <v>92.26694884007246</v>
       </c>
       <c r="Y117">
-        <v>0</v>
+        <v>76.10312044039974</v>
       </c>
       <c r="Z117">
-        <v>17.99302549252018</v>
+        <v>85.36061992768661</v>
       </c>
     </row>
     <row r="118" spans="1:26">
@@ -11375,10 +11375,10 @@
         <v>92.50041558493287</v>
       </c>
       <c r="Y118">
-        <v>0</v>
+        <v>76.72214487820365</v>
       </c>
       <c r="Z118">
-        <v>18.97289315739902</v>
+        <v>85.58001586212271</v>
       </c>
     </row>
     <row r="119" spans="1:26">
@@ -11455,10 +11455,10 @@
         <v>92.69274614459897</v>
       </c>
       <c r="Y119">
-        <v>0</v>
+        <v>77.13276240110403</v>
       </c>
       <c r="Z119">
-        <v>22.54263674552278</v>
+        <v>86.37929443644971</v>
       </c>
     </row>
     <row r="120" spans="1:26">
@@ -11535,10 +11535,10 @@
         <v>92.85118859944879</v>
       </c>
       <c r="Y120">
-        <v>0</v>
+        <v>77.56060833376391</v>
       </c>
       <c r="Z120">
-        <v>26.37484426682742</v>
+        <v>87.23733964012879</v>
       </c>
     </row>
     <row r="121" spans="1:26">
@@ -11615,10 +11615,10 @@
         <v>92.98171393844025</v>
       </c>
       <c r="Y121">
-        <v>0</v>
+        <v>78.01481551814437</v>
       </c>
       <c r="Z121">
-        <v>26.42500863758001</v>
+        <v>87.24857162521312</v>
       </c>
     </row>
     <row r="122" spans="1:26">
@@ -11695,10 +11695,10 @@
         <v>93.08924107903515</v>
       </c>
       <c r="Y122">
-        <v>0.7903754256831985</v>
+        <v>78.65286906743184</v>
       </c>
       <c r="Z122">
-        <v>27.621335890404</v>
+        <v>87.51643364876216</v>
       </c>
     </row>
     <row r="123" spans="1:26">
@@ -11775,10 +11775,10 @@
         <v>93.17782223924398</v>
       </c>
       <c r="Y123">
-        <v>1.779105412167725</v>
+        <v>78.9579230068685</v>
       </c>
       <c r="Z123">
-        <v>29.09890340070163</v>
+        <v>87.84726638897118</v>
       </c>
     </row>
     <row r="124" spans="1:26">
@@ -11855,10 +11855,10 @@
         <v>93.25079564763679</v>
       </c>
       <c r="Y124">
-        <v>2.949867081279134</v>
+        <v>79.31913937957484</v>
       </c>
       <c r="Z124">
-        <v>29.12851682665727</v>
+        <v>87.85389694276159</v>
       </c>
     </row>
     <row r="125" spans="1:26">
@@ -11935,10 +11935,10 @@
         <v>93.31091134627869</v>
       </c>
       <c r="Y125">
-        <v>2.097400807526206</v>
+        <v>79.05612703181568</v>
       </c>
       <c r="Z125">
-        <v>31.31555293279937</v>
+        <v>88.34358228227276</v>
       </c>
     </row>
   </sheetData>
@@ -17766,7 +17766,7 @@
         <v>23</v>
       </c>
       <c r="B416">
-        <v>2.097400807526206</v>
+        <v>79.05612703181568</v>
       </c>
       <c r="C416" t="s">
         <v>477</v>
@@ -17780,7 +17780,7 @@
         <v>420</v>
       </c>
       <c r="B417">
-        <v>51.50079930119757</v>
+        <v>94.298611368351</v>
       </c>
       <c r="C417" t="s">
         <v>477</v>
@@ -17794,7 +17794,7 @@
         <v>421</v>
       </c>
       <c r="B418">
-        <v>34.319869181793</v>
+        <v>88.9977602889321</v>
       </c>
       <c r="C418" t="s">
         <v>477</v>
@@ -17808,7 +17808,7 @@
         <v>422</v>
       </c>
       <c r="B419">
-        <v>63.48604912037641</v>
+        <v>97.99643354675186</v>
       </c>
       <c r="C419" t="s">
         <v>477</v>
@@ -17822,7 +17822,7 @@
         <v>423</v>
       </c>
       <c r="B420">
-        <v>18.51306389857069</v>
+        <v>84.1208694416143</v>
       </c>
       <c r="C420" t="s">
         <v>477</v>
@@ -17836,7 +17836,7 @@
         <v>424</v>
       </c>
       <c r="B421">
-        <v>51.89221645435443</v>
+        <v>94.41937572885954</v>
       </c>
       <c r="C421" t="s">
         <v>477</v>
@@ -17850,7 +17850,7 @@
         <v>425</v>
       </c>
       <c r="B422">
-        <v>48.94929697910534</v>
+        <v>93.5113935783821</v>
       </c>
       <c r="C422" t="s">
         <v>477</v>
@@ -17864,7 +17864,7 @@
         <v>426</v>
       </c>
       <c r="B423">
-        <v>10.60294797504787</v>
+        <v>81.68035276177646</v>
       </c>
       <c r="C423" t="s">
         <v>477</v>
@@ -17878,7 +17878,7 @@
         <v>427</v>
       </c>
       <c r="B424">
-        <v>30.46076216421878</v>
+        <v>87.80710579831188</v>
       </c>
       <c r="C424" t="s">
         <v>477</v>
@@ -17892,7 +17892,7 @@
         <v>428</v>
       </c>
       <c r="B425">
-        <v>30.93665667476256</v>
+        <v>87.95393404988934</v>
       </c>
       <c r="C425" t="s">
         <v>477</v>
@@ -17906,7 +17906,7 @@
         <v>429</v>
       </c>
       <c r="B426">
-        <v>10.12135163962732</v>
+        <v>81.53176531996081</v>
       </c>
       <c r="C426" t="s">
         <v>477</v>
@@ -17920,7 +17920,7 @@
         <v>430</v>
       </c>
       <c r="B427">
-        <v>40.56658917335149</v>
+        <v>90.92506761047665</v>
       </c>
       <c r="C427" t="s">
         <v>477</v>
@@ -17934,7 +17934,7 @@
         <v>431</v>
       </c>
       <c r="B428">
-        <v>55.38171556382328</v>
+        <v>95.49599468909639</v>
       </c>
       <c r="C428" t="s">
         <v>477</v>
@@ -17948,7 +17948,7 @@
         <v>432</v>
       </c>
       <c r="B429">
-        <v>6.515603783682222</v>
+        <v>80.41928000738091</v>
       </c>
       <c r="C429" t="s">
         <v>477</v>
@@ -17962,7 +17962,7 @@
         <v>433</v>
       </c>
       <c r="B430">
-        <v>57.01648051326556</v>
+        <v>96.00037049917314</v>
       </c>
       <c r="C430" t="s">
         <v>477</v>
@@ -17976,7 +17976,7 @@
         <v>434</v>
       </c>
       <c r="B431">
-        <v>66.77254632849923</v>
+        <v>99.01042010930171</v>
       </c>
       <c r="C431" t="s">
         <v>477</v>
@@ -17990,7 +17990,7 @@
         <v>435</v>
       </c>
       <c r="B432">
-        <v>35.35394991336936</v>
+        <v>89.3168063431383</v>
       </c>
       <c r="C432" t="s">
         <v>477</v>
@@ -18004,7 +18004,7 @@
         <v>436</v>
       </c>
       <c r="B433">
-        <v>8.031411302155444</v>
+        <v>80.8869537517388</v>
       </c>
       <c r="C433" t="s">
         <v>477</v>
@@ -18018,7 +18018,7 @@
         <v>24</v>
       </c>
       <c r="B434">
-        <v>31.31555293279937</v>
+        <v>88.34358228227276</v>
       </c>
       <c r="C434" t="s">
         <v>478</v>
@@ -18032,7 +18032,7 @@
         <v>437</v>
       </c>
       <c r="B435">
-        <v>62.19312157792293</v>
+        <v>95.25718221910445</v>
       </c>
       <c r="C435" t="s">
         <v>478</v>
@@ -18046,7 +18046,7 @@
         <v>438</v>
       </c>
       <c r="B436">
-        <v>59.13087894925255</v>
+        <v>94.5715349556348</v>
       </c>
       <c r="C436" t="s">
         <v>478</v>
@@ -18060,7 +18060,7 @@
         <v>439</v>
       </c>
       <c r="B437">
-        <v>57.98867538730899</v>
+        <v>94.31579142334773</v>
       </c>
       <c r="C437" t="s">
         <v>478</v>
@@ -18074,7 +18074,7 @@
         <v>440</v>
       </c>
       <c r="B438">
-        <v>36.82096901627136</v>
+        <v>89.5762649693192</v>
       </c>
       <c r="C438" t="s">
         <v>478</v>
@@ -18088,7 +18088,7 @@
         <v>441</v>
       </c>
       <c r="B439">
-        <v>68.64771055581011</v>
+        <v>96.70238816982784</v>
       </c>
       <c r="C439" t="s">
         <v>478</v>
@@ -18102,7 +18102,7 @@
         <v>442</v>
       </c>
       <c r="B440">
-        <v>62.92066434380494</v>
+        <v>95.42008169082334</v>
       </c>
       <c r="C440" t="s">
         <v>478</v>
@@ -18116,7 +18116,7 @@
         <v>443</v>
       </c>
       <c r="B441">
-        <v>39.12737632543865</v>
+        <v>90.09267795540045</v>
       </c>
       <c r="C441" t="s">
         <v>478</v>
@@ -18130,7 +18130,7 @@
         <v>444</v>
       </c>
       <c r="B442">
-        <v>61.8395088729032</v>
+        <v>95.17800704818436</v>
       </c>
       <c r="C442" t="s">
         <v>478</v>
@@ -18144,7 +18144,7 @@
         <v>445</v>
       </c>
       <c r="B443">
-        <v>52.76560843681632</v>
+        <v>93.14632773422167</v>
       </c>
       <c r="C443" t="s">
         <v>478</v>
@@ -18158,7 +18158,7 @@
         <v>446</v>
       </c>
       <c r="B444">
-        <v>34.2749737213428</v>
+        <v>89.00620736172428</v>
       </c>
       <c r="C444" t="s">
         <v>478</v>
@@ -18172,7 +18172,7 @@
         <v>447</v>
       </c>
       <c r="B445">
-        <v>62.16119921442144</v>
+        <v>95.25003468579897</v>
       </c>
       <c r="C445" t="s">
         <v>478</v>
@@ -18186,7 +18186,7 @@
         <v>448</v>
       </c>
       <c r="B446">
-        <v>65.21723068674252</v>
+        <v>95.93429124876933</v>
       </c>
       <c r="C446" t="s">
         <v>478</v>
@@ -18200,7 +18200,7 @@
         <v>449</v>
       </c>
       <c r="B447">
-        <v>44.07005747071184</v>
+        <v>91.19936224283526</v>
       </c>
       <c r="C447" t="s">
         <v>478</v>
@@ -18214,7 +18214,7 @@
         <v>450</v>
       </c>
       <c r="B448">
-        <v>64.86062790214081</v>
+        <v>95.85444658815429</v>
       </c>
       <c r="C448" t="s">
         <v>478</v>
@@ -18228,7 +18228,7 @@
         <v>451</v>
       </c>
       <c r="B449">
-        <v>67.47407942214039</v>
+        <v>96.43960788991484</v>
       </c>
       <c r="C449" t="s">
         <v>478</v>
@@ -18242,7 +18242,7 @@
         <v>452</v>
       </c>
       <c r="B450">
-        <v>64.02343850861874</v>
+        <v>95.66699683766704</v>
       </c>
       <c r="C450" t="s">
         <v>478</v>
@@ -18256,7 +18256,7 @@
         <v>453</v>
       </c>
       <c r="B451">
-        <v>49.99880370872837</v>
+        <v>92.52683009134813</v>
       </c>
       <c r="C451" t="s">
         <v>478</v>

</xml_diff>